<commit_message>
ShopSpellTable 에 type|String 컬럼 제거 ShopActorTable 추가
</commit_message>
<xml_diff>
--- a/Excel/Gacha.xlsx
+++ b/Excel/Gacha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0B0268-BB81-4BB0-9E8E-4EE17449AA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B8BB87-5948-465C-8447-93F9B49A27F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2730" windowWidth="28830" windowHeight="7830" activeTab="2" xr2:uid="{46033DEB-6FD4-418A-B621-781919E55E75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{46033DEB-6FD4-418A-B621-781919E55E75}"/>
   </bookViews>
   <sheets>
     <sheet name="GachaSpellTable" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>grade|Int</t>
   </si>
@@ -73,10 +73,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>type|String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>count|Int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -89,10 +85,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Spell</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Spell10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -105,15 +97,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Actor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Actor10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Actor50</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -598,18 +582,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19FFAC4-D517-4B5B-AF66-D461905177C5}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -619,49 +601,37 @@
       <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
+      <c r="B4">
+        <v>50</v>
       </c>
       <c r="C4">
-        <v>50</v>
-      </c>
-      <c r="D4">
         <v>400000</v>
       </c>
     </row>
@@ -675,7 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BEF23C-412E-4D28-AEE8-44AC7F89AF56}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -689,10 +659,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -703,7 +673,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -714,7 +684,7 @@
         <v>0.04</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -725,7 +695,7 @@
         <v>0.16</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -736,17 +706,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE6DDCC6-F5B0-489A-9DF2-62AB0ECF9CDA}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -756,50 +725,27 @@
       <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
         <v>90000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>50</v>
-      </c>
-      <c r="D4">
-        <v>400000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
가챠 엑셀에 GachaEquipTable, ShopEquipTable 시트 추가
</commit_message>
<xml_diff>
--- a/Excel/Gacha.xlsx
+++ b/Excel/Gacha.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFB59FF-9752-4CCB-8FD0-5A7D1211543B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62031D7-14F9-45E7-BD5C-3ECA442300C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{46033DEB-6FD4-418A-B621-781919E55E75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="2" activeTab="5" xr2:uid="{46033DEB-6FD4-418A-B621-781919E55E75}"/>
   </bookViews>
   <sheets>
     <sheet name="GachaSpellTable" sheetId="1" r:id="rId1"/>
     <sheet name="ShopSpellTable" sheetId="2" r:id="rId2"/>
     <sheet name="GachaActorTable" sheetId="5" r:id="rId3"/>
     <sheet name="ShopActorTable" sheetId="3" r:id="rId4"/>
+    <sheet name="GachaEquipTable" sheetId="6" r:id="rId5"/>
+    <sheet name="ShopEquipTable" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>grade|Int</t>
   </si>
@@ -121,6 +123,15 @@
   </si>
   <si>
     <t>Actor10</t>
+  </si>
+  <si>
+    <t>prob|float</t>
+  </si>
+  <si>
+    <t>Equip1</t>
+  </si>
+  <si>
+    <t>Equip10</t>
   </si>
 </sst>
 </file>
@@ -713,7 +724,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE6DDCC6-F5B0-489A-9DF2-62AB0ECF9CDA}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -758,4 +771,118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE98F16-E941-497F-9DA3-F4E03C58161F}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.34899999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96048EF0-3537-4B44-944F-0B06AC9FD7C7}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>750000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ShopEquipTable, GachaEquipTable 엑셀 올림
</commit_message>
<xml_diff>
--- a/Excel/Gacha.xlsx
+++ b/Excel/Gacha.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectNameless\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1D7C9B-90F3-41DB-BFD7-4619C7B48815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF7FF27-F43D-440C-9DA9-E913BBC62BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{46033DEB-6FD4-418A-B621-781919E55E75}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{46033DEB-6FD4-418A-B621-781919E55E75}"/>
   </bookViews>
   <sheets>
     <sheet name="GachaSpellTable" sheetId="1" r:id="rId1"/>
     <sheet name="ShopSpellTable" sheetId="2" r:id="rId2"/>
     <sheet name="GachaActorTable" sheetId="5" r:id="rId3"/>
     <sheet name="ShopActorTable" sheetId="3" r:id="rId4"/>
-    <sheet name="GachaEquipTable" sheetId="6" r:id="rId5"/>
-    <sheet name="ShopEquipTable" sheetId="7" r:id="rId6"/>
+    <sheet name="ShopEquipTable" sheetId="7" r:id="rId5"/>
+    <sheet name="GachaEquipTable" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>grade|Int</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Equip10</t>
   </si>
   <si>
-    <t>Equip50</t>
-  </si>
-  <si>
     <t>Spell2</t>
   </si>
   <si>
@@ -120,6 +117,12 @@
   </si>
   <si>
     <t>1, 0.75, 0.67, 0.45, 0.33, 0.22, 0.16, 0.12, 0.1, 0.08, 0.06, 0.042, 0.042, 0.042, 0.042, 0.042, 0.042, 0.042, 0.042, 0.042, 0.042</t>
+  </si>
+  <si>
+    <t>Equip20</t>
+  </si>
+  <si>
+    <t>rarity|Int</t>
   </si>
 </sst>
 </file>
@@ -590,7 +593,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19FFAC4-D517-4B5B-AF66-D461905177C5}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -610,7 +615,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -621,7 +626,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -632,7 +637,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -679,7 +684,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -690,7 +695,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -701,7 +706,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -764,72 +769,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE98F16-E941-497F-9DA3-F4E03C58161F}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>4.4999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>0.34899999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96048EF0-3537-4B44-944F-0B06AC9FD7C7}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -873,13 +816,106 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
         <v>20</v>
       </c>
+      <c r="C4">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE98F16-E941-497F-9DA3-F4E03C58161F}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>800</v>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>